<commit_message>
[ADD] Added xml2json and now we get the videos from Kaltura server
</commit_message>
<xml_diff>
--- a/2019_05.xlsx
+++ b/2019_05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ruymy\Documents\UPM\TFG\StorageCSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC20A134-CC61-460E-9D2D-87B1F97D7FB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5208CC6-AA11-43AD-93B5-E9EC7F233CEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A0371084-3A69-4FBF-931F-C13DD5562A6A}"/>
+    <workbookView xWindow="0" yWindow="4245" windowWidth="21600" windowHeight="11505" xr2:uid="{A0371084-3A69-4FBF-931F-C13DD5562A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
-  <si>
-    <t>Miniatura</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Subtitulo</t>
   </si>
@@ -45,9 +42,6 @@
     <t>Campus Sur Radio</t>
   </si>
   <si>
-    <t>mp4</t>
-  </si>
-  <si>
     <t>Ejemplo de vídeo 2</t>
   </si>
   <si>
@@ -63,40 +57,58 @@
     <t>Timestamp_inicio</t>
   </si>
   <si>
-    <t>Tipo_de_archivo</t>
-  </si>
-  <si>
     <t>Estudio</t>
   </si>
   <si>
-    <t>Audio 1</t>
-  </si>
-  <si>
-    <t>Subtitulo audio</t>
-  </si>
-  <si>
-    <t>Miniatura_audio.jpg</t>
-  </si>
-  <si>
-    <t>audio.mp3</t>
-  </si>
-  <si>
-    <t>mp3</t>
-  </si>
-  <si>
     <t>Podcast de prueba de vídeo</t>
   </si>
   <si>
     <t>Podcast de vídeo</t>
   </si>
   <si>
-    <t>thumb.jpg</t>
-  </si>
-  <si>
-    <t>2019_05_15_01.mp4</t>
-  </si>
-  <si>
     <t>Duracion</t>
+  </si>
+  <si>
+    <t>0_c58wk4db</t>
+  </si>
+  <si>
+    <t>Ejemplo de vídeo 3</t>
+  </si>
+  <si>
+    <t>Subtítulo 3</t>
+  </si>
+  <si>
+    <t>Ejemplo de vídeo 4</t>
+  </si>
+  <si>
+    <t>Subtítulo 4</t>
+  </si>
+  <si>
+    <t>Ejemplo de vídeo 5</t>
+  </si>
+  <si>
+    <t>Subtítulo 5</t>
+  </si>
+  <si>
+    <t>0_sr0gkznr</t>
+  </si>
+  <si>
+    <t>0_hvo9z7lv</t>
+  </si>
+  <si>
+    <t>0_5r02f10i</t>
+  </si>
+  <si>
+    <t>0_97s649gx</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Esto es un audio</t>
+  </si>
+  <si>
+    <t>0_8ba2t465</t>
   </si>
 </sst>
 </file>
@@ -480,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB13E14-7F9E-42A8-A641-C8B96DF34335}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,36 +508,30 @@
     <col min="11" max="11" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1557853200000</v>
       </c>
@@ -533,83 +539,134 @@
         <v>1557856800000</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>127</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>127</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1558023276000</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>127</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>130</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1558023276000</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1558023276000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>127</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1558109676000</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1558109677500</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1558091306400</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1558089866400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>250</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>